<commit_message>
update script SP Gerencia OK
se elimino el nombre de la base de datos que aparecia por delante del nombre de las tablas
</commit_message>
<xml_diff>
--- a/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_10_casos.xlsx
+++ b/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_10_casos.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Edad</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Tipo de Proyecto</t>
+  </si>
+  <si>
+    <t>1a</t>
   </si>
 </sst>
 </file>
@@ -650,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AD10" sqref="AD10"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AG3" sqref="AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,10 +888,12 @@
       <c r="AF2" s="2">
         <v>4</v>
       </c>
-      <c r="AG2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="14"/>
+      <c r="AG2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH2" s="14">
+        <v>44479</v>
+      </c>
       <c r="AI2" s="2">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
update script variable Es Adulto OK
</commit_message>
<xml_diff>
--- a/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_10_casos.xlsx
+++ b/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_10_casos.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Edad</t>
   </si>
@@ -163,9 +163,6 @@
   </si>
   <si>
     <t>Tipo de Proyecto</t>
-  </si>
-  <si>
-    <t>1a</t>
   </si>
 </sst>
 </file>
@@ -653,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AG3" sqref="AG3"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,13 +853,13 @@
         <v>1</v>
       </c>
       <c r="V2" s="2">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="W2" s="2">
         <v>1</v>
       </c>
       <c r="X2" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Y2" s="3">
         <v>1</v>
@@ -888,8 +885,8 @@
       <c r="AF2" s="2">
         <v>4</v>
       </c>
-      <c r="AG2" s="2" t="s">
-        <v>42</v>
+      <c r="AG2" s="2">
+        <v>1</v>
       </c>
       <c r="AH2" s="14">
         <v>44479</v>
@@ -947,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="V3" s="2">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="W3" s="2">
         <v>2</v>

</xml_diff>